<commit_message>
best NN Model found, new mode tested
</commit_message>
<xml_diff>
--- a/dis/ml_results.xlsx
+++ b/dis/ml_results.xlsx
@@ -5,13 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NB" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="conf_matrix" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name=" GB" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="NN" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="conf_matrix" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name=" GB" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="short_circuit" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
   <si>
     <t xml:space="preserve">n_feats</t>
   </si>
@@ -55,9 +57,18 @@
     <t xml:space="preserve">BEST NB</t>
   </si>
   <si>
+    <t xml:space="preserve">BEST_GB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEST_NN</t>
+  </si>
+  <si>
     <t xml:space="preserve">Depth 3</t>
   </si>
   <si>
+    <t xml:space="preserve">Глубина 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Параметр</t>
   </si>
   <si>
@@ -70,22 +81,225 @@
     <t xml:space="preserve">n_params</t>
   </si>
   <si>
+    <t xml:space="preserve">Гиперпараметр</t>
+  </si>
+  <si>
     <t xml:space="preserve"> n_estimators</t>
   </si>
   <si>
+    <t xml:space="preserve">n_estimators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Количество деревьев, используемых в ансамбле </t>
+  </si>
+  <si>
     <t xml:space="preserve">max_depth</t>
   </si>
   <si>
+    <t xml:space="preserve">Максимальная «глубина» каждого решающего дерева</t>
+  </si>
+  <si>
     <t xml:space="preserve">learning_rate</t>
   </si>
   <si>
+    <t xml:space="preserve">Скорость обучения, определяет размер шага на каждой итерации</t>
+  </si>
+  <si>
     <t xml:space="preserve">loss_function</t>
   </si>
   <si>
+    <t xml:space="preserve">Функция потерь (стоимости), в данной работе используется «Multiclass»</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random_state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Фиксация ГПСЧ для возможности повторения эксперимента</t>
+  </si>
+  <si>
+    <t xml:space="preserve">l2_leaf_reg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коэффициент L2 регуляризации в функции стоимости</t>
+  </si>
+  <si>
     <t xml:space="preserve">Depth 5</t>
   </si>
   <si>
-    <t xml:space="preserve">Depth 7</t>
+    <t xml:space="preserve">Глубина 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Параметры модели</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Средняя точность</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точность по классам</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_estimators=300,
+max_depth=4,
+learning_rate=0.5,
+loss_function='MultiClass'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_estimators=300,
+max_depth=4,
+learning_rate=0.55,
+loss_function='MultiClass'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_estimators=500,
+max_depth=2,
+learning_rate=0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_estimators=500,
+max_depth=3,
+Learning_rate=0.7,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_estimators=300,
+max_depth=3,
+learning_rate=0.7,
+class_weights=[1.7,1,1],
+l2_leaf_reg=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Идентификатор режима</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Метка класса</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Предсказанное занчение</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(le_8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(more_20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(more_8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">more_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3011e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0011701</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.998817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000378624</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.9995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000121681</t>
+  </si>
+  <si>
+    <t xml:space="preserve">le_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999856</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000120333</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.32924e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.73519e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999839</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0001439</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.78606e-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.494097</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505895</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0571581</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.94279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.18593e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.85761e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.999762</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.000159682</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.85637e-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.49913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.500863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.18303e-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.681348</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.31863</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.79118e-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.494422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.505571</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Точность</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Средняя точность в классе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Наивный Байесовкий классификатор</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Градиентный бустинг</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Искуственная нейросеть</t>
   </si>
   <si>
     <t xml:space="preserve">Стратегия классификации</t>
@@ -153,11 +367,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -175,154 +390,37 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -333,7 +431,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,89 +455,70 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -447,45 +526,28 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
@@ -497,7 +559,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -513,7 +575,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -535,7 +597,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -574,6 +636,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -703,6 +766,7 @@
           </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -802,17 +866,17 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="4964573"/>
-        <c:axId val="46220429"/>
+        <c:axId val="68542403"/>
+        <c:axId val="12998898"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="4964573"/>
+        <c:axId val="68542403"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -834,12 +898,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46220429"/>
+        <c:crossAx val="12998898"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46220429"/>
+        <c:axId val="12998898"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -854,7 +918,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -876,7 +940,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4964573"/>
+        <c:crossAx val="68542403"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -924,7 +988,502 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.121835344127024"/>
+          <c:y val="0.0418010005558644"/>
+          <c:w val="0.689504282052885"/>
+          <c:h val="0.810894941634241"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>' GB'!$C$12:$C$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Глубина 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>' GB'!$B$14:$B$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>155</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>' GB'!$C$14:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>71.34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>69.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>65.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68.4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>64.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>69.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>69.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70.1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>59.6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>61.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>' GB'!$H$2:$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Глубина 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="r"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>' GB'!$G$4:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>' GB'!$H$4:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>71.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>77.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71.9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>68.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>61.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>63.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="63945480"/>
+        <c:axId val="44555104"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="63945480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="ru-RU" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="ru-RU" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t> Количество признаков</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="ru-RU" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="44555104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="44555104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="55"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" lang="ru-RU" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" lang="ru-RU" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Точность</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" lang="ru-RU" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="63945480"/>
+        <c:crossesAt val="0"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" lang="ru-RU" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="span"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -936,9 +1495,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.0721971971971972"/>
-          <c:y val="0.0199578778457527"/>
-          <c:w val="0.812374874874875"/>
-          <c:h val="0.636646274195166"/>
+          <c:y val="0.0199618818336844"/>
+          <c:w val="0.81224974974975"/>
+          <c:h val="0.636573377470157"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -950,7 +1509,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>Sheet1!$C$2:$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -970,6 +1529,7 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1033,7 +1593,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>Sheet1!$E$2:$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1053,6 +1613,7 @@
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1113,11 +1674,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="4922849"/>
-        <c:axId val="10987145"/>
+        <c:axId val="72059967"/>
+        <c:axId val="62724"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="4922849"/>
+        <c:axId val="72059967"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1145,14 +1706,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10987145"/>
+        <c:crossAx val="62724"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10987145"/>
+        <c:axId val="62724"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1167,7 +1728,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1189,7 +1750,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4922849"/>
+        <c:crossAx val="72059967"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1247,9 +1808,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>423360</xdr:colOff>
+      <xdr:colOff>422640</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1258,7 +1819,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="2791440" y="294120"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1273,6 +1834,379 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>583920</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>37440</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Image 6" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2091600" y="229320"/>
+          <a:ext cx="4994640" cy="3546720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>117720</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 7" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438280" y="4226400"/>
+          <a:ext cx="4994640" cy="3546720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>207720</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>132840</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 8" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438280" y="8452800"/>
+          <a:ext cx="5897160" cy="5497560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>673920</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>207720</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>75960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 9" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="673920" y="14505840"/>
+          <a:ext cx="6036120" cy="4589640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>811080</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>88560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152280</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 1" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5987520" y="9716760"/>
+          <a:ext cx="5030640" cy="3544200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>226440</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>115200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>340920</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>365040</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 2" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6215760" y="6001560"/>
+          <a:ext cx="4991040" cy="3544200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>961560</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>414000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>75240</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>42120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 4" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11827440" y="10042200"/>
+          <a:ext cx="5052240" cy="3573000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1178640</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>480600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1399680</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1883880</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 5" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId4"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12044520" y="1882440"/>
+          <a:ext cx="1514520" cy="1403280"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>619920</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>57240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>666720</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>64080</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="3335760" y="3687840"/>
+        <a:ext cx="5758560" cy="3237840"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>753840</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>615600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>411480</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Image 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId6"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11619720" y="6048720"/>
+          <a:ext cx="4987440" cy="3543480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1282,18 +2216,18 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>531360</xdr:colOff>
+      <xdr:colOff>530640</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>51120</xdr:rowOff>
+      <xdr:rowOff>50400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvPr id="11" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="851760" y="2176200"/>
-        <a:ext cx="5753880" cy="3589200"/>
+        <a:ext cx="5753880" cy="3588480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1482,10 +2416,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E95" activeCellId="0" sqref="E95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E30" activeCellId="0" sqref="E30"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1669,12 +2630,164 @@
         <v>0.311111111111111</v>
       </c>
     </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5"/>
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>64</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5"/>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5"/>
+      <c r="B29" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="E29" s="3" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5"/>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3" t="n">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="8">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="C10:E10"/>
     <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="A28:A30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1686,41 +2799,49 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:I29"/>
+  <dimension ref="B2:M73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.69"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.28"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G2" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
         <v>1</v>
@@ -1728,10 +2849,16 @@
       <c r="I3" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>60</v>
@@ -1742,10 +2869,16 @@
       <c r="I4" s="0" t="n">
         <v>69</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>65</v>
@@ -1756,24 +2889,36 @@
       <c r="I5" s="0" t="n">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>70</v>
       </c>
       <c r="H6" s="0" t="n">
-        <v>71.3</v>
+        <v>78.4</v>
       </c>
       <c r="I6" s="0" t="n">
-        <v>70.5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78.1</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="151.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>75</v>
@@ -1784,8 +2929,14 @@
       <c r="I7" s="0" t="n">
         <v>65.2</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G8" s="0" t="n">
         <v>80</v>
       </c>
@@ -1795,8 +2946,14 @@
       <c r="I8" s="0" t="n">
         <v>65.8</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G9" s="0" t="n">
         <v>85</v>
       </c>
@@ -1805,29 +2962,56 @@
       </c>
       <c r="I9" s="0" t="n">
         <v>59.1</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G10" s="0" t="n">
         <v>90</v>
       </c>
+      <c r="H10" s="0" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>76.2</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G11" s="0" t="n">
         <v>100</v>
       </c>
+      <c r="H11" s="0" t="n">
+        <v>70.8</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>68</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>20</v>
+        <v>32</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="0" t="n">
+        <v>150</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>71.9</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>1</v>
@@ -1835,14 +3019,14 @@
       <c r="D13" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>2</v>
+      <c r="G13" s="0" t="n">
+        <v>200</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>68.4</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>65.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,6 +3039,15 @@
       <c r="D14" s="0" t="n">
         <v>68.7</v>
       </c>
+      <c r="G14" s="0" t="n">
+        <v>250</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>61.4</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>52.7</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="n">
@@ -1866,6 +3059,15 @@
       <c r="D15" s="0" t="n">
         <v>65.2</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>300</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>63.7</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>55.4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="n">
@@ -1927,10 +3129,10 @@
         <v>149</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>70.1</v>
+        <v>73.7</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,6 +3221,343 @@
       </c>
       <c r="D29" s="0" t="n">
         <v>63.7</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3" t="n">
+        <v>73.1</v>
+      </c>
+      <c r="D35" s="3" t="n">
+        <v>69.9</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="3" t="n">
+        <v>73.7</v>
+      </c>
+      <c r="D36" s="3" t="n">
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="3" t="n">
+        <v>74.9</v>
+      </c>
+      <c r="D37" s="3" t="n">
+        <v>73.7</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="3" t="n">
+        <v>78.9</v>
+      </c>
+      <c r="D38" s="3" t="n">
+        <v>78.9</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="57.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" s="3" t="n">
+        <v>78.4</v>
+      </c>
+      <c r="D39" s="3" t="n">
+        <v>76.1</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D63" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I63" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C64" s="12"/>
+      <c r="D64" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F64" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I64" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="J64" s="11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C65" s="12"/>
+      <c r="D65" s="11" t="n">
+        <v>39</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F65" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C66" s="12"/>
+      <c r="D66" s="11" t="n">
+        <v>107</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F66" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H66" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I66" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J66" s="11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="12"/>
+      <c r="D67" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F67" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H67" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="I67" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J67" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="12"/>
+      <c r="D68" s="11" t="n">
+        <v>67</v>
+      </c>
+      <c r="E68" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F68" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H68" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I68" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J68" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="12"/>
+      <c r="D69" s="11" t="n">
+        <v>147</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F69" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H69" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I69" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J69" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="12"/>
+      <c r="D70" s="11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F70" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H70" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I70" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="J70" s="11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C71" s="12"/>
+      <c r="D71" s="11" t="n">
+        <v>65</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F71" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="12"/>
+      <c r="D72" s="11" t="n">
+        <v>36</v>
+      </c>
+      <c r="E72" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F72" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H72" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I72" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J72" s="11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C73" s="12"/>
+      <c r="D73" s="11" t="n">
+        <v>64</v>
+      </c>
+      <c r="E73" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F73" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J73" s="11" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2029,10 +3568,84 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B3:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="3" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1"/>
+      <c r="C3" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="14" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="D4" s="14" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="14" t="n">
+        <v>0.57</v>
+      </c>
+      <c r="D5" s="14" t="n">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="14" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="D6" s="14" t="n">
+        <v>0.576</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2052,50 +3665,50 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.72"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="6" t="s">
-        <v>21</v>
+      <c r="B2" s="15" t="s">
+        <v>87</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7" t="s">
-        <v>23</v>
+        <v>89</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="8"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6" t="s">
-        <v>24</v>
+      <c r="B3" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="I3" s="6"/>
+        <v>92</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="I3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>27</v>
+        <v>93</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="C4" s="7" t="n">
         <v>50.2</v>
@@ -2109,17 +3722,17 @@
       <c r="F4" s="7" t="n">
         <v>50.9</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="I4" s="6" t="s">
-        <v>27</v>
+      <c r="G4" s="16"/>
+      <c r="I4" s="15" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>94</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="C5" s="7" t="n">
         <v>75.4</v>
@@ -2133,17 +3746,17 @@
       <c r="F5" s="7" t="n">
         <v>71.2</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
+      <c r="G5" s="16"/>
+      <c r="I5" s="15" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>31</v>
+      <c r="B6" s="15" t="s">
+        <v>97</v>
       </c>
       <c r="C6" s="7" t="n">
         <v>56.7</v>
@@ -2157,17 +3770,17 @@
       <c r="F6" s="7" t="n">
         <v>41</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="I6" s="6" t="s">
-        <v>32</v>
+      <c r="G6" s="16"/>
+      <c r="I6" s="15" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>34</v>
+        <v>99</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>100</v>
       </c>
       <c r="C7" s="7" t="n">
         <v>63.1</v>
@@ -2181,17 +3794,17 @@
       <c r="F7" s="7" t="n">
         <v>56</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="I7" s="6" t="s">
-        <v>34</v>
+      <c r="G7" s="16"/>
+      <c r="I7" s="15" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>36</v>
+        <v>101</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C8" s="7" t="n">
         <v>63.7</v>
@@ -2205,14 +3818,14 @@
       <c r="F8" s="7" t="n">
         <v>67.4</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="I8" s="6" t="s">
-        <v>37</v>
+      <c r="G8" s="16"/>
+      <c r="I8" s="15" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>38</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>